<commit_message>
Bug fix data (cats platform) and hydrogen plus storage model
</commit_message>
<xml_diff>
--- a/Data/OurData3FullCheck.xlsx
+++ b/Data/OurData3FullCheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E62A577-884C-9049-877C-3F2198EC9961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9576CE5B-2CA7-234B-84E1-27CD476830A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="22060" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" activeTab="2" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -2137,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
   <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5929,7 +5929,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6450,10 +6450,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B95C95-5100-B242-B62A-0A2629824349}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6480,173 +6480,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="13">
-        <v>0.12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="13">
-        <v>0</v>
-      </c>
-      <c r="B3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="13">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
-        <v>0</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="13">
-        <v>0</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="C5" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="B6" s="13">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="B7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
-        <v>0.15</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="B10" s="13">
-        <v>0</v>
-      </c>
-      <c r="C10" s="13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="B11" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" s="13">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="C13" s="13">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
-        <v>0.45</v>
-      </c>
-      <c r="B14" s="13">
-        <v>0</v>
-      </c>
-      <c r="C14" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="13">
-        <v>0.45</v>
-      </c>
-      <c r="B15" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="13">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="13">
-        <v>0.45</v>
-      </c>
-      <c r="B16" s="13">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="13">
-        <v>0.45</v>
-      </c>
-      <c r="B17" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="C17" s="13">
-        <v>0.12</v>
-      </c>
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6659,7 +6502,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7798,10 +7641,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2444F6-F631-0348-A27B-77CDC677869C}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="A16:H16"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8256,6 +8099,160 @@
       <c r="H24">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J39" s="13">
+        <v>0</v>
+      </c>
+      <c r="K39" s="13">
+        <v>1</v>
+      </c>
+      <c r="L39" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J40" s="13">
+        <v>0</v>
+      </c>
+      <c r="K40" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="L40" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J41" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="K41" s="13">
+        <v>0</v>
+      </c>
+      <c r="L41" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J42" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="K42" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L42" s="13">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="43" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J43" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="K43" s="13">
+        <v>1</v>
+      </c>
+      <c r="L43" s="13">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="44" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J44" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="K44" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="L44" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J45" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="K45" s="13">
+        <v>0</v>
+      </c>
+      <c r="L45" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="46" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J46" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="K46" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L46" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J47" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="K47" s="13">
+        <v>1</v>
+      </c>
+      <c r="L47" s="13">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="48" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J48" s="13">
+        <v>0.3</v>
+      </c>
+      <c r="K48" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="49" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J49" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="K49" s="13">
+        <v>0</v>
+      </c>
+      <c r="L49" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J50" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="K50" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="L50" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="51" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J51" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="K51" s="13">
+        <v>1</v>
+      </c>
+      <c r="L51" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="10:12" x14ac:dyDescent="0.2">
+      <c r="J52" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="K52" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="L52" s="13">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>
@@ -8390,7 +8387,7 @@
   <dimension ref="A1:AI64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8656,7 +8653,8 @@
         <v>10</v>
       </c>
       <c r="AB3" s="3">
-        <v>0</v>
+        <f>N3</f>
+        <v>100</v>
       </c>
       <c r="AC3" s="3">
         <f>O3</f>
@@ -8769,34 +8767,35 @@
         <v>10</v>
       </c>
       <c r="AB4" s="3">
-        <v>0</v>
+        <f t="shared" ref="AB4:AB61" si="3">N4</f>
+        <v>100</v>
       </c>
       <c r="AC4" s="3">
-        <f t="shared" ref="AC4:AC61" si="3">O4</f>
+        <f t="shared" ref="AC4:AC61" si="4">O4</f>
         <v>2</v>
       </c>
       <c r="AD4" s="3">
-        <f t="shared" ref="AD4:AD61" si="4">P4</f>
+        <f t="shared" ref="AD4:AD61" si="5">P4</f>
         <v>5</v>
       </c>
       <c r="AE4" s="3">
-        <f t="shared" ref="AE4:AE61" si="5">Q4</f>
+        <f t="shared" ref="AE4:AE61" si="6">Q4</f>
         <v>5</v>
       </c>
       <c r="AF4" s="3">
-        <f t="shared" ref="AF4:AF61" si="6">R4</f>
+        <f t="shared" ref="AF4:AF61" si="7">R4</f>
         <v>5.2</v>
       </c>
       <c r="AG4" s="3">
-        <f t="shared" ref="AG4:AG61" si="7">S4</f>
+        <f t="shared" ref="AG4:AG61" si="8">S4</f>
         <v>5.2</v>
       </c>
       <c r="AH4" s="3">
-        <f t="shared" ref="AH4:AH61" si="8">T4</f>
+        <f t="shared" ref="AH4:AH61" si="9">T4</f>
         <v>5.4</v>
       </c>
       <c r="AI4" s="3">
-        <f t="shared" ref="AI4:AI61" si="9">U4</f>
+        <f t="shared" ref="AI4:AI61" si="10">U4</f>
         <v>5.4</v>
       </c>
     </row>
@@ -8884,34 +8883,35 @@
         <v>10</v>
       </c>
       <c r="AB5" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC5" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE5" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF5" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG5" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG5" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH5" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI5" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -8997,34 +8997,35 @@
         <v>10</v>
       </c>
       <c r="AB6" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC6" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE6" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF6" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG6" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG6" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH6" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI6" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9110,34 +9111,35 @@
         <v>10</v>
       </c>
       <c r="AB7" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC7" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE7" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF7" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG7" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG7" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH7" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI7" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9225,34 +9227,35 @@
         <v>10</v>
       </c>
       <c r="AB8" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE8" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF8" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG8" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG8" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH8" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI8" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9340,34 +9343,35 @@
         <v>10</v>
       </c>
       <c r="AB9" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE9" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF9" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG9" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG9" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH9" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI9" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9453,34 +9457,35 @@
         <v>10</v>
       </c>
       <c r="AB10" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC10" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE10" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF10" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG10" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG10" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH10" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI10" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9566,34 +9571,35 @@
         <v>10</v>
       </c>
       <c r="AB11" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC11" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE11" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF11" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG11" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG11" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH11" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI11" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9679,34 +9685,35 @@
         <v>10</v>
       </c>
       <c r="AB12" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD12" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE12" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF12" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG12" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG12" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH12" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI12" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9792,34 +9799,35 @@
         <v>10</v>
       </c>
       <c r="AB13" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD13" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF13" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG13" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG13" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI13" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -9905,34 +9913,35 @@
         <v>10</v>
       </c>
       <c r="AB14" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD14" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF14" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG14" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG14" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI14" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10020,34 +10029,35 @@
         <v>10</v>
       </c>
       <c r="AB15" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD15" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF15" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG15" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG15" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI15" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10133,34 +10143,35 @@
         <v>10</v>
       </c>
       <c r="AB16" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD16" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF16" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG16" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG16" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI16" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10246,34 +10257,35 @@
         <v>10</v>
       </c>
       <c r="AB17" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD17" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF17" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG17" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG17" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI17" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10359,34 +10371,35 @@
         <v>10</v>
       </c>
       <c r="AB18" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD18" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF18" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG18" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG18" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI18" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10474,34 +10487,35 @@
         <v>10</v>
       </c>
       <c r="AB19" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF19" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG19" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG19" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI19" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10589,34 +10603,35 @@
         <v>10</v>
       </c>
       <c r="AB20" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD20" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF20" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG20" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG20" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH20" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI20" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10704,34 +10719,35 @@
         <v>10</v>
       </c>
       <c r="AB21" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD21" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF21" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG21" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG21" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI21" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10817,34 +10833,35 @@
         <v>10</v>
       </c>
       <c r="AB22" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF22" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG22" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG22" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI22" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -10932,34 +10949,35 @@
         <v>10</v>
       </c>
       <c r="AB23" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD23" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF23" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG23" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG23" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI23" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11047,34 +11065,35 @@
         <v>10</v>
       </c>
       <c r="AB24" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD24" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF24" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG24" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG24" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH24" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI24" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11160,34 +11179,35 @@
         <v>10</v>
       </c>
       <c r="AB25" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD25" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF25" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG25" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG25" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI25" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11273,34 +11293,35 @@
         <v>10</v>
       </c>
       <c r="AB26" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD26" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF26" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG26" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG26" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI26" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11388,34 +11409,35 @@
         <v>10</v>
       </c>
       <c r="AB27" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD27" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF27" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG27" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG27" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11503,34 +11525,35 @@
         <v>10</v>
       </c>
       <c r="AB28" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF28" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG28" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG28" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11618,34 +11641,35 @@
         <v>10</v>
       </c>
       <c r="AB29" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF29" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG29" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG29" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11731,34 +11755,35 @@
         <v>10</v>
       </c>
       <c r="AB30" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF30" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG30" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG30" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11844,34 +11869,35 @@
         <v>10</v>
       </c>
       <c r="AB31" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE31" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF31" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG31" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG31" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -11957,34 +11983,35 @@
         <v>10</v>
       </c>
       <c r="AB32" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE32" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF32" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG32" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG32" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12072,34 +12099,35 @@
         <v>10</v>
       </c>
       <c r="AB33" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE33" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF33" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG33" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG33" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI33" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12185,34 +12213,35 @@
         <v>10</v>
       </c>
       <c r="AB34" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE34" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF34" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG34" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG34" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI34" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12298,34 +12327,35 @@
         <v>10</v>
       </c>
       <c r="AB35" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE35" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF35" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG35" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG35" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI35" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12413,34 +12443,35 @@
         <v>10</v>
       </c>
       <c r="AB36" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE36" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF36" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG36" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG36" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI36" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12528,34 +12559,35 @@
         <v>10</v>
       </c>
       <c r="AB37" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE37" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF37" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG37" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG37" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH37" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI37" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12641,34 +12673,35 @@
         <v>10</v>
       </c>
       <c r="AB38" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE38" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF38" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG38" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG38" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH38" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI38" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12754,34 +12787,35 @@
         <v>10</v>
       </c>
       <c r="AB39" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE39" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF39" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG39" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG39" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH39" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI39" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12867,34 +12901,35 @@
         <v>10</v>
       </c>
       <c r="AB40" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC40" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD40" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE40" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF40" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG40" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG40" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH40" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI40" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -12982,34 +13017,35 @@
         <v>10</v>
       </c>
       <c r="AB41" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC41" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD41" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE41" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF41" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG41" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG41" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH41" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI41" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13095,34 +13131,35 @@
         <v>10</v>
       </c>
       <c r="AB42" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC42" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD42" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE42" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF42" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG42" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG42" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH42" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI42" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13210,34 +13247,35 @@
         <v>10</v>
       </c>
       <c r="AB43" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC43" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD43" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE43" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF43" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG43" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG43" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH43" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI43" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13325,34 +13363,35 @@
         <v>10</v>
       </c>
       <c r="AB44" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC44" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD44" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE44" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF44" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG44" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG44" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH44" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI44" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13438,34 +13477,35 @@
         <v>10</v>
       </c>
       <c r="AB45" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC45" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD45" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE45" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF45" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG45" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG45" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH45" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI45" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13551,34 +13591,35 @@
         <v>10</v>
       </c>
       <c r="AB46" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC46" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD46" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE46" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF46" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG46" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG46" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH46" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI46" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13664,34 +13705,35 @@
         <v>10</v>
       </c>
       <c r="AB47" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC47" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD47" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE47" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF47" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG47" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG47" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH47" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI47" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13777,34 +13819,35 @@
         <v>10</v>
       </c>
       <c r="AB48" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC48" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD48" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE48" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF48" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG48" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG48" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH48" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI48" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -13892,34 +13935,35 @@
         <v>10</v>
       </c>
       <c r="AB49" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC49" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD49" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE49" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF49" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG49" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG49" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH49" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI49" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14007,34 +14051,35 @@
         <v>10</v>
       </c>
       <c r="AB50" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC50" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD50" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE50" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF50" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG50" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG50" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH50" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI50" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14122,34 +14167,35 @@
         <v>10</v>
       </c>
       <c r="AB51" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC51" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD51" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE51" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF51" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG51" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG51" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH51" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI51" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14235,34 +14281,35 @@
         <v>10</v>
       </c>
       <c r="AB52" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC52" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD52" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE52" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF52" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG52" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG52" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH52" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI52" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14348,34 +14395,35 @@
         <v>10</v>
       </c>
       <c r="AB53" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC53" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD53" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE53" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF53" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG53" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG53" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH53" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI53" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14463,34 +14511,35 @@
         <v>10</v>
       </c>
       <c r="AB54" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC54" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD54" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE54" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF54" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG54" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG54" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH54" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI54" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14576,34 +14625,35 @@
         <v>10</v>
       </c>
       <c r="AB55" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC55" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD55" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE55" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF55" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG55" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG55" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH55" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI55" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14689,34 +14739,35 @@
         <v>10</v>
       </c>
       <c r="AB56" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC56" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD56" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE56" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF56" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG56" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG56" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH56" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI56" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14804,34 +14855,35 @@
         <v>10</v>
       </c>
       <c r="AB57" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC57" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD57" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE57" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF57" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG57" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG57" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH57" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI57" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -14919,34 +14971,35 @@
         <v>10</v>
       </c>
       <c r="AB58" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD58" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE58" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF58" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG58" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG58" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH58" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI58" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -15032,34 +15085,35 @@
         <v>10</v>
       </c>
       <c r="AB59" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC59" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD59" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE59" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF59" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG59" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG59" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH59" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI59" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -15147,34 +15201,35 @@
         <v>10</v>
       </c>
       <c r="AB60" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC60" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9990000000000001</v>
       </c>
       <c r="AD60" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE60" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF60" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG60" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG60" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH60" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI60" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -15260,34 +15315,35 @@
         <v>10</v>
       </c>
       <c r="AB61" s="3">
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>100</v>
       </c>
       <c r="AC61" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="AD61" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="AE61" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AF61" s="3">
-        <f t="shared" si="6"/>
-        <v>5.2</v>
-      </c>
-      <c r="AG61" s="3">
         <f t="shared" si="7"/>
         <v>5.2</v>
       </c>
+      <c r="AG61" s="3">
+        <f t="shared" si="8"/>
+        <v>5.2</v>
+      </c>
       <c r="AH61" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AI61" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.4</v>
       </c>
     </row>
@@ -16306,7 +16362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19292E87-5CF7-794D-A1AA-7C1926221C7B}">
   <dimension ref="A1:BM58"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="AL2" zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="BE38" sqref="BE38"/>
     </sheetView>
   </sheetViews>
@@ -34511,7 +34567,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34612,7 +34668,7 @@
         <v>342</v>
       </c>
       <c r="B12">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>